<commit_message>
Can Forecast Room Nights Sold
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/JASON/ForecastResult2017.xlsx
+++ b/Prototype/PHPSCRIPTS/JASON/ForecastResult2017.xlsx
@@ -9,13 +9,16 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="rns">'Sheet1'!$C$2:$C$7</definedName>
+    <definedName name="Timeline">'Sheet1'!$B$2:$B$7</definedName>
+  </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -26,85 +29,10 @@
     <t>Room Nights Sold</t>
   </si>
   <si>
-    <t>Forecast</t>
+    <t>Forecasted Date</t>
   </si>
   <si>
-    <t>Lower Confidence Bound</t>
-  </si>
-  <si>
-    <t>Upper Confidence Bound</t>
-  </si>
-  <si>
-    <t>2015-01-31</t>
-  </si>
-  <si>
-    <t>2015-02-28</t>
-  </si>
-  <si>
-    <t>2015-03-31</t>
-  </si>
-  <si>
-    <t>2015-04-30</t>
-  </si>
-  <si>
-    <t>2015-05-31</t>
-  </si>
-  <si>
-    <t>2015-06-30</t>
-  </si>
-  <si>
-    <t>2015-07-31</t>
-  </si>
-  <si>
-    <t>2015-08-31</t>
-  </si>
-  <si>
-    <t>2015-09-30</t>
-  </si>
-  <si>
-    <t>2015-10-31</t>
-  </si>
-  <si>
-    <t>2015-11-30</t>
-  </si>
-  <si>
-    <t>2015-12-31</t>
-  </si>
-  <si>
-    <t>2016-01-31</t>
-  </si>
-  <si>
-    <t>2016-02-28</t>
-  </si>
-  <si>
-    <t>2016-03-31</t>
-  </si>
-  <si>
-    <t>2016-04-30</t>
-  </si>
-  <si>
-    <t>2016-05-31</t>
-  </si>
-  <si>
-    <t>2016-06-30</t>
-  </si>
-  <si>
-    <t>2016-07-31</t>
-  </si>
-  <si>
-    <t>2016-08-31</t>
-  </si>
-  <si>
-    <t>2016-09-30</t>
-  </si>
-  <si>
-    <t>2016-10-31</t>
-  </si>
-  <si>
-    <t>2016-11-30</t>
-  </si>
-  <si>
-    <t>2016-12-31</t>
+    <t>Forecast</t>
   </si>
 </sst>
 </file>
@@ -454,10 +382,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G335"/>
+  <dimension ref="A1:G362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,7 +394,7 @@
     <col min="3" max="3" width="19.28515625" customWidth="true" style="0"/>
     <col min="5" max="5" width="25.42578125" customWidth="true" style="0"/>
     <col min="6" max="6" width="24" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15.85546875" customWidth="true" style="0"/>
+    <col min="7" max="7" width="23.5703125" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -479,222 +407,132 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="2" t="s">
-        <v>6</v>
+      <c r="B2" s="2" t="str">
+        <f>DATE(2016,07,31)</f>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1072</v>
-      </c>
+        <v>1100</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>EOMONTH(DATE(2016,12,31),1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>_xlfn.FORECAST.ETS($E2,rns,Timeline,1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="2" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="str">
+        <f>DATE(2016,08,31)</f>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>578</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="2" t="s">
-        <v>8</v>
+      <c r="B4" s="2" t="str">
+        <f>DATE(2016,09,30)</f>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>447</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+      <c r="B5" s="2" t="str">
+        <f>DATE(2016,10,31)</f>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1074</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+      <c r="B6" s="2" t="str">
+        <f>DATE(2016,11,30)</f>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>955</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="B7" s="2" t="s">
-        <v>11</v>
+      <c r="B7" s="2" t="str">
+        <f>DATE(2016,12,31)</f>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>590</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>467</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>831</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>467</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>636</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>1088</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>1402</v>
-      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>1072</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>1186</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>1268</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>734</v>
-      </c>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>798</v>
-      </c>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="B19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19">
-        <v>791</v>
-      </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>1100</v>
-      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="B21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21">
-        <v>1003</v>
-      </c>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22">
-        <v>1223</v>
-      </c>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="B23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <v>1440</v>
-      </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="B24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24">
-        <v>1161</v>
-      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="B25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25">
-        <v>2686</v>
-      </c>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="2"/>
-      <c r="D26" t="str">
-        <f>FORECAST.ETS(B26,$C$2:$C$25,$B$2:$B$25,1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" t="str">
-        <f>FORECAST.ETS(B26,$C$2:$C$25,$B$2:$B$25,1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" t="str">
-        <f>FORECAST.ETS(B26,$C$2:$C$25,$B$2:$B$25,1,1)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="2"/>
@@ -1622,6 +1460,87 @@
     </row>
     <row r="335" spans="1:7">
       <c r="B335" s="2"/>
+    </row>
+    <row r="336" spans="1:7">
+      <c r="B336" s="2"/>
+    </row>
+    <row r="337" spans="1:7">
+      <c r="B337" s="2"/>
+    </row>
+    <row r="338" spans="1:7">
+      <c r="B338" s="2"/>
+    </row>
+    <row r="339" spans="1:7">
+      <c r="B339" s="2"/>
+    </row>
+    <row r="340" spans="1:7">
+      <c r="B340" s="2"/>
+    </row>
+    <row r="341" spans="1:7">
+      <c r="B341" s="2"/>
+    </row>
+    <row r="342" spans="1:7">
+      <c r="B342" s="2"/>
+    </row>
+    <row r="343" spans="1:7">
+      <c r="B343" s="2"/>
+    </row>
+    <row r="344" spans="1:7">
+      <c r="B344" s="2"/>
+    </row>
+    <row r="345" spans="1:7">
+      <c r="B345" s="2"/>
+    </row>
+    <row r="346" spans="1:7">
+      <c r="B346" s="2"/>
+    </row>
+    <row r="347" spans="1:7">
+      <c r="B347" s="2"/>
+    </row>
+    <row r="348" spans="1:7">
+      <c r="B348" s="2"/>
+    </row>
+    <row r="349" spans="1:7">
+      <c r="B349" s="2"/>
+    </row>
+    <row r="350" spans="1:7">
+      <c r="B350" s="2"/>
+    </row>
+    <row r="351" spans="1:7">
+      <c r="B351" s="2"/>
+    </row>
+    <row r="352" spans="1:7">
+      <c r="B352" s="2"/>
+    </row>
+    <row r="353" spans="1:7">
+      <c r="B353" s="2"/>
+    </row>
+    <row r="354" spans="1:7">
+      <c r="B354" s="2"/>
+    </row>
+    <row r="355" spans="1:7">
+      <c r="B355" s="2"/>
+    </row>
+    <row r="356" spans="1:7">
+      <c r="B356" s="2"/>
+    </row>
+    <row r="357" spans="1:7">
+      <c r="B357" s="2"/>
+    </row>
+    <row r="358" spans="1:7">
+      <c r="B358" s="2"/>
+    </row>
+    <row r="359" spans="1:7">
+      <c r="B359" s="2"/>
+    </row>
+    <row r="360" spans="1:7">
+      <c r="B360" s="2"/>
+    </row>
+    <row r="361" spans="1:7">
+      <c r="B361" s="2"/>
+    </row>
+    <row r="362" spans="1:7">
+      <c r="B362" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Removed ID from Forecast Template
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/JASON/ForecastResult2017.xlsx
+++ b/Prototype/PHPSCRIPTS/JASON/ForecastResult2017.xlsx
@@ -10,18 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="rns">'Sheet1'!$C$2:$C$7</definedName>
-    <definedName name="Timeline">'Sheet1'!$B$2:$B$7</definedName>
+    <definedName name="rns">'Sheet1'!$B$2:$B$7</definedName>
+    <definedName name="Timeline">'Sheet1'!$A$2:$A$7</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Timeline</t>
   </si>
@@ -382,1171 +379,1028 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G362"/>
+  <dimension ref="A1:G315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="11" customWidth="true" style="0"/>
+    <col min="1" max="1" width="12.5703125" customWidth="true" style="0"/>
+    <col min="2" max="2" width="16.7109375" customWidth="true" style="0"/>
     <col min="3" max="3" width="19.28515625" customWidth="true" style="0"/>
-    <col min="5" max="5" width="25.42578125" customWidth="true" style="0"/>
-    <col min="6" max="6" width="24" customWidth="true" style="0"/>
-    <col min="7" max="7" width="23.5703125" customWidth="true" style="0"/>
+    <col min="4" max="4" width="15.42578125" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10.85546875" customWidth="true" style="0"/>
+    <col min="6" max="6" width="7.42578125" customWidth="true" style="0"/>
+    <col min="7" max="7" width="8" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="2" t="str">
+      <c r="A2" s="2" t="str">
         <f>DATE(2016,07,31)</f>
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>1100</v>
       </c>
-      <c r="E2" s="2" t="str">
+      <c r="D2" t="str">
         <f>EOMONTH(DATE(2016,12,31),1)</f>
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="str">
-        <f>_xlfn.FORECAST.ETS($E2,rns,Timeline,1,1)</f>
+      <c r="E2" t="str">
+        <f>_xlfn.FORECAST.ETS($D2,rns,timeline,1,1)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="2" t="str">
+      <c r="A3" s="2" t="str">
         <f>DATE(2016,08,31)</f>
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>1003</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="2" t="str">
+      <c r="A4" s="2" t="str">
         <f>DATE(2016,09,30)</f>
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>1223</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="B5" s="2" t="str">
+      <c r="A5" s="2" t="str">
         <f>DATE(2016,10,31)</f>
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="B5">
         <v>1440</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="B6" s="2" t="str">
+      <c r="A6" s="2" t="str">
         <f>DATE(2016,11,30)</f>
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="B6">
         <v>1161</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="B7" s="2" t="str">
+      <c r="A7" s="2" t="str">
         <f>DATE(2016,12,31)</f>
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="B7">
         <v>2686</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="2"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="2"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="2"/>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" s="2"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="B12" s="2"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="2"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="B14" s="2"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="2"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" s="2"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="2"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="2"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="B19" s="2"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" s="2"/>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="B21" s="2"/>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="B22" s="2"/>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="B23" s="2"/>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="B24" s="2"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="B25" s="2"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="B26" s="2"/>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="B27" s="2"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="B28" s="2"/>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" s="2"/>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="B30" s="2"/>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="B31" s="2"/>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" s="2"/>
+      <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="B33" s="2"/>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="B34" s="2"/>
+      <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="B35" s="2"/>
+      <c r="A35" s="2"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="B36" s="2"/>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="B37" s="2"/>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="B38" s="2"/>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="B39" s="2"/>
+      <c r="A39" s="2"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="B40" s="2"/>
+      <c r="A40" s="2"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="B41" s="2"/>
+      <c r="A41" s="2"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="B42" s="2"/>
+      <c r="A42" s="2"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="B43" s="2"/>
+      <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="B44" s="2"/>
+      <c r="A44" s="2"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="B45" s="2"/>
+      <c r="A45" s="2"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="B46" s="2"/>
+      <c r="A46" s="2"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="B47" s="2"/>
+      <c r="A47" s="2"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="B48" s="2"/>
+      <c r="A48" s="2"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="B49" s="2"/>
+      <c r="A49" s="2"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="B50" s="2"/>
+      <c r="A50" s="2"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="B51" s="2"/>
+      <c r="A51" s="2"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="B52" s="2"/>
+      <c r="A52" s="2"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="B53" s="2"/>
+      <c r="A53" s="2"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="B54" s="2"/>
+      <c r="A54" s="2"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="B55" s="2"/>
+      <c r="A55" s="2"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="B56" s="2"/>
+      <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="B57" s="2"/>
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="B58" s="2"/>
+      <c r="A58" s="2"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="B59" s="2"/>
+      <c r="A59" s="2"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="B60" s="2"/>
+      <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="B61" s="2"/>
+      <c r="A61" s="2"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="B62" s="2"/>
+      <c r="A62" s="2"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="B63" s="2"/>
+      <c r="A63" s="2"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="B64" s="2"/>
+      <c r="A64" s="2"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="B65" s="2"/>
+      <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="B66" s="2"/>
+      <c r="A66" s="2"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="B67" s="2"/>
+      <c r="A67" s="2"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="B68" s="2"/>
+      <c r="A68" s="2"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="B69" s="2"/>
+      <c r="A69" s="2"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="B70" s="2"/>
+      <c r="A70" s="2"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="B71" s="2"/>
+      <c r="A71" s="2"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="B72" s="2"/>
+      <c r="A72" s="2"/>
     </row>
     <row r="73" spans="1:7">
-      <c r="B73" s="2"/>
+      <c r="A73" s="2"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="B74" s="2"/>
+      <c r="A74" s="2"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="B75" s="2"/>
+      <c r="A75" s="2"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="B76" s="2"/>
+      <c r="A76" s="2"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="B77" s="2"/>
+      <c r="A77" s="2"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="B78" s="2"/>
+      <c r="A78" s="2"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="B79" s="2"/>
+      <c r="A79" s="2"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="B80" s="2"/>
+      <c r="A80" s="2"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="B81" s="2"/>
+      <c r="A81" s="2"/>
     </row>
     <row r="82" spans="1:7">
-      <c r="B82" s="2"/>
+      <c r="A82" s="2"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="B83" s="2"/>
+      <c r="A83" s="2"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="B84" s="2"/>
+      <c r="A84" s="2"/>
     </row>
     <row r="85" spans="1:7">
-      <c r="B85" s="2"/>
+      <c r="A85" s="2"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="B86" s="2"/>
+      <c r="A86" s="2"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="B87" s="2"/>
+      <c r="A87" s="2"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="B88" s="2"/>
+      <c r="A88" s="2"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="B89" s="2"/>
+      <c r="A89" s="2"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="B90" s="2"/>
+      <c r="A90" s="2"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="B91" s="2"/>
+      <c r="A91" s="2"/>
     </row>
     <row r="92" spans="1:7">
-      <c r="B92" s="2"/>
+      <c r="A92" s="2"/>
     </row>
     <row r="93" spans="1:7">
-      <c r="B93" s="2"/>
+      <c r="A93" s="2"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="B94" s="2"/>
+      <c r="A94" s="2"/>
     </row>
     <row r="95" spans="1:7">
-      <c r="B95" s="2"/>
+      <c r="A95" s="2"/>
     </row>
     <row r="96" spans="1:7">
-      <c r="B96" s="2"/>
+      <c r="A96" s="2"/>
     </row>
     <row r="97" spans="1:7">
-      <c r="B97" s="2"/>
+      <c r="A97" s="2"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="B98" s="2"/>
+      <c r="A98" s="2"/>
     </row>
     <row r="99" spans="1:7">
-      <c r="B99" s="2"/>
+      <c r="A99" s="2"/>
     </row>
     <row r="100" spans="1:7">
-      <c r="B100" s="2"/>
+      <c r="A100" s="2"/>
     </row>
     <row r="101" spans="1:7">
-      <c r="B101" s="2"/>
+      <c r="A101" s="2"/>
     </row>
     <row r="102" spans="1:7">
-      <c r="B102" s="2"/>
+      <c r="A102" s="2"/>
     </row>
     <row r="103" spans="1:7">
-      <c r="B103" s="2"/>
+      <c r="A103" s="2"/>
     </row>
     <row r="104" spans="1:7">
-      <c r="B104" s="2"/>
+      <c r="A104" s="2"/>
     </row>
     <row r="105" spans="1:7">
-      <c r="B105" s="2"/>
+      <c r="A105" s="2"/>
     </row>
     <row r="106" spans="1:7">
-      <c r="B106" s="2"/>
+      <c r="A106" s="2"/>
     </row>
     <row r="107" spans="1:7">
-      <c r="B107" s="2"/>
+      <c r="A107" s="2"/>
     </row>
     <row r="108" spans="1:7">
-      <c r="B108" s="2"/>
+      <c r="A108" s="2"/>
     </row>
     <row r="109" spans="1:7">
-      <c r="B109" s="2"/>
+      <c r="A109" s="2"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="B110" s="2"/>
+      <c r="A110" s="2"/>
     </row>
     <row r="111" spans="1:7">
-      <c r="B111" s="2"/>
+      <c r="A111" s="2"/>
     </row>
     <row r="112" spans="1:7">
-      <c r="B112" s="2"/>
+      <c r="A112" s="2"/>
     </row>
     <row r="113" spans="1:7">
-      <c r="B113" s="2"/>
+      <c r="A113" s="2"/>
     </row>
     <row r="114" spans="1:7">
-      <c r="B114" s="2"/>
+      <c r="A114" s="2"/>
     </row>
     <row r="115" spans="1:7">
-      <c r="B115" s="2"/>
+      <c r="A115" s="2"/>
     </row>
     <row r="116" spans="1:7">
-      <c r="B116" s="2"/>
+      <c r="A116" s="2"/>
     </row>
     <row r="117" spans="1:7">
-      <c r="B117" s="2"/>
+      <c r="A117" s="2"/>
     </row>
     <row r="118" spans="1:7">
-      <c r="B118" s="2"/>
+      <c r="A118" s="2"/>
     </row>
     <row r="119" spans="1:7">
-      <c r="B119" s="2"/>
+      <c r="A119" s="2"/>
     </row>
     <row r="120" spans="1:7">
-      <c r="B120" s="2"/>
+      <c r="A120" s="2"/>
     </row>
     <row r="121" spans="1:7">
-      <c r="B121" s="2"/>
+      <c r="A121" s="2"/>
     </row>
     <row r="122" spans="1:7">
-      <c r="B122" s="2"/>
+      <c r="A122" s="2"/>
     </row>
     <row r="123" spans="1:7">
-      <c r="B123" s="2"/>
+      <c r="A123" s="2"/>
     </row>
     <row r="124" spans="1:7">
-      <c r="B124" s="2"/>
+      <c r="A124" s="2"/>
     </row>
     <row r="125" spans="1:7">
-      <c r="B125" s="2"/>
+      <c r="A125" s="2"/>
     </row>
     <row r="126" spans="1:7">
-      <c r="B126" s="2"/>
+      <c r="A126" s="2"/>
     </row>
     <row r="127" spans="1:7">
-      <c r="B127" s="2"/>
+      <c r="A127" s="2"/>
     </row>
     <row r="128" spans="1:7">
-      <c r="B128" s="2"/>
+      <c r="A128" s="2"/>
     </row>
     <row r="129" spans="1:7">
-      <c r="B129" s="2"/>
+      <c r="A129" s="2"/>
     </row>
     <row r="130" spans="1:7">
-      <c r="B130" s="2"/>
+      <c r="A130" s="2"/>
     </row>
     <row r="131" spans="1:7">
-      <c r="B131" s="2"/>
+      <c r="A131" s="2"/>
     </row>
     <row r="132" spans="1:7">
-      <c r="B132" s="2"/>
+      <c r="A132" s="2"/>
     </row>
     <row r="133" spans="1:7">
-      <c r="B133" s="2"/>
+      <c r="A133" s="2"/>
     </row>
     <row r="134" spans="1:7">
-      <c r="B134" s="2"/>
+      <c r="A134" s="2"/>
     </row>
     <row r="135" spans="1:7">
-      <c r="B135" s="2"/>
+      <c r="A135" s="2"/>
     </row>
     <row r="136" spans="1:7">
-      <c r="B136" s="2"/>
+      <c r="A136" s="2"/>
     </row>
     <row r="137" spans="1:7">
-      <c r="B137" s="2"/>
+      <c r="A137" s="2"/>
     </row>
     <row r="138" spans="1:7">
-      <c r="B138" s="2"/>
+      <c r="A138" s="2"/>
     </row>
     <row r="139" spans="1:7">
-      <c r="B139" s="2"/>
+      <c r="A139" s="2"/>
     </row>
     <row r="140" spans="1:7">
-      <c r="B140" s="2"/>
+      <c r="A140" s="2"/>
     </row>
     <row r="141" spans="1:7">
-      <c r="B141" s="2"/>
+      <c r="A141" s="2"/>
     </row>
     <row r="142" spans="1:7">
-      <c r="B142" s="2"/>
+      <c r="A142" s="2"/>
     </row>
     <row r="143" spans="1:7">
-      <c r="B143" s="2"/>
+      <c r="A143" s="2"/>
     </row>
     <row r="144" spans="1:7">
-      <c r="B144" s="2"/>
+      <c r="A144" s="2"/>
     </row>
     <row r="145" spans="1:7">
-      <c r="B145" s="2"/>
+      <c r="A145" s="2"/>
     </row>
     <row r="146" spans="1:7">
-      <c r="B146" s="2"/>
+      <c r="A146" s="2"/>
     </row>
     <row r="147" spans="1:7">
-      <c r="B147" s="2"/>
+      <c r="A147" s="2"/>
     </row>
     <row r="148" spans="1:7">
-      <c r="B148" s="2"/>
+      <c r="A148" s="2"/>
     </row>
     <row r="149" spans="1:7">
-      <c r="B149" s="2"/>
+      <c r="A149" s="2"/>
     </row>
     <row r="150" spans="1:7">
-      <c r="B150" s="2"/>
+      <c r="A150" s="2"/>
     </row>
     <row r="151" spans="1:7">
-      <c r="B151" s="2"/>
+      <c r="A151" s="2"/>
     </row>
     <row r="152" spans="1:7">
-      <c r="B152" s="2"/>
+      <c r="A152" s="2"/>
     </row>
     <row r="153" spans="1:7">
-      <c r="B153" s="2"/>
+      <c r="A153" s="2"/>
     </row>
     <row r="154" spans="1:7">
-      <c r="B154" s="2"/>
+      <c r="A154" s="2"/>
     </row>
     <row r="155" spans="1:7">
-      <c r="B155" s="2"/>
+      <c r="A155" s="2"/>
     </row>
     <row r="156" spans="1:7">
-      <c r="B156" s="2"/>
+      <c r="A156" s="2"/>
     </row>
     <row r="157" spans="1:7">
-      <c r="B157" s="2"/>
+      <c r="A157" s="2"/>
     </row>
     <row r="158" spans="1:7">
-      <c r="B158" s="2"/>
+      <c r="A158" s="2"/>
     </row>
     <row r="159" spans="1:7">
-      <c r="B159" s="2"/>
+      <c r="A159" s="2"/>
     </row>
     <row r="160" spans="1:7">
-      <c r="B160" s="2"/>
+      <c r="A160" s="2"/>
     </row>
     <row r="161" spans="1:7">
-      <c r="B161" s="2"/>
+      <c r="A161" s="2"/>
     </row>
     <row r="162" spans="1:7">
-      <c r="B162" s="2"/>
+      <c r="A162" s="2"/>
     </row>
     <row r="163" spans="1:7">
-      <c r="B163" s="2"/>
+      <c r="A163" s="2"/>
     </row>
     <row r="164" spans="1:7">
-      <c r="B164" s="2"/>
+      <c r="A164" s="2"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="B165" s="2"/>
+      <c r="A165" s="2"/>
     </row>
     <row r="166" spans="1:7">
-      <c r="B166" s="2"/>
+      <c r="A166" s="2"/>
     </row>
     <row r="167" spans="1:7">
-      <c r="B167" s="2"/>
+      <c r="A167" s="2"/>
     </row>
     <row r="168" spans="1:7">
-      <c r="B168" s="2"/>
+      <c r="A168" s="2"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="B169" s="2"/>
+      <c r="A169" s="2"/>
     </row>
     <row r="170" spans="1:7">
-      <c r="B170" s="2"/>
+      <c r="A170" s="2"/>
     </row>
     <row r="171" spans="1:7">
-      <c r="B171" s="2"/>
+      <c r="A171" s="2"/>
     </row>
     <row r="172" spans="1:7">
-      <c r="B172" s="2"/>
+      <c r="A172" s="2"/>
     </row>
     <row r="173" spans="1:7">
-      <c r="B173" s="2"/>
+      <c r="A173" s="2"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="B174" s="2"/>
+      <c r="A174" s="2"/>
     </row>
     <row r="175" spans="1:7">
-      <c r="B175" s="2"/>
+      <c r="A175" s="2"/>
     </row>
     <row r="176" spans="1:7">
-      <c r="B176" s="2"/>
+      <c r="A176" s="2"/>
     </row>
     <row r="177" spans="1:7">
-      <c r="B177" s="2"/>
+      <c r="A177" s="2"/>
     </row>
     <row r="178" spans="1:7">
-      <c r="B178" s="2"/>
+      <c r="A178" s="2"/>
     </row>
     <row r="179" spans="1:7">
-      <c r="B179" s="2"/>
+      <c r="A179" s="2"/>
     </row>
     <row r="180" spans="1:7">
-      <c r="B180" s="2"/>
+      <c r="A180" s="2"/>
     </row>
     <row r="181" spans="1:7">
-      <c r="B181" s="2"/>
+      <c r="A181" s="2"/>
     </row>
     <row r="182" spans="1:7">
-      <c r="B182" s="2"/>
+      <c r="A182" s="2"/>
     </row>
     <row r="183" spans="1:7">
-      <c r="B183" s="2"/>
+      <c r="A183" s="2"/>
     </row>
     <row r="184" spans="1:7">
-      <c r="B184" s="2"/>
+      <c r="A184" s="2"/>
     </row>
     <row r="185" spans="1:7">
-      <c r="B185" s="2"/>
+      <c r="A185" s="2"/>
     </row>
     <row r="186" spans="1:7">
-      <c r="B186" s="2"/>
+      <c r="A186" s="2"/>
     </row>
     <row r="187" spans="1:7">
-      <c r="B187" s="2"/>
+      <c r="A187" s="2"/>
     </row>
     <row r="188" spans="1:7">
-      <c r="B188" s="2"/>
+      <c r="A188" s="2"/>
     </row>
     <row r="189" spans="1:7">
-      <c r="B189" s="2"/>
+      <c r="A189" s="2"/>
     </row>
     <row r="190" spans="1:7">
-      <c r="B190" s="2"/>
+      <c r="A190" s="2"/>
     </row>
     <row r="191" spans="1:7">
-      <c r="B191" s="2"/>
+      <c r="A191" s="2"/>
     </row>
     <row r="192" spans="1:7">
-      <c r="B192" s="2"/>
+      <c r="A192" s="2"/>
     </row>
     <row r="193" spans="1:7">
-      <c r="B193" s="2"/>
+      <c r="A193" s="2"/>
     </row>
     <row r="194" spans="1:7">
-      <c r="B194" s="2"/>
+      <c r="A194" s="2"/>
     </row>
     <row r="195" spans="1:7">
-      <c r="B195" s="2"/>
+      <c r="A195" s="2"/>
     </row>
     <row r="196" spans="1:7">
-      <c r="B196" s="2"/>
+      <c r="A196" s="2"/>
     </row>
     <row r="197" spans="1:7">
-      <c r="B197" s="2"/>
+      <c r="A197" s="2"/>
     </row>
     <row r="198" spans="1:7">
-      <c r="B198" s="2"/>
+      <c r="A198" s="2"/>
     </row>
     <row r="199" spans="1:7">
-      <c r="B199" s="2"/>
+      <c r="A199" s="2"/>
     </row>
     <row r="200" spans="1:7">
-      <c r="B200" s="2"/>
+      <c r="A200" s="2"/>
     </row>
     <row r="201" spans="1:7">
-      <c r="B201" s="2"/>
+      <c r="A201" s="2"/>
     </row>
     <row r="202" spans="1:7">
-      <c r="B202" s="2"/>
+      <c r="A202" s="2"/>
     </row>
     <row r="203" spans="1:7">
-      <c r="B203" s="2"/>
+      <c r="A203" s="2"/>
     </row>
     <row r="204" spans="1:7">
-      <c r="B204" s="2"/>
+      <c r="A204" s="2"/>
     </row>
     <row r="205" spans="1:7">
-      <c r="B205" s="2"/>
+      <c r="A205" s="2"/>
     </row>
     <row r="206" spans="1:7">
-      <c r="B206" s="2"/>
+      <c r="A206" s="2"/>
     </row>
     <row r="207" spans="1:7">
-      <c r="B207" s="2"/>
+      <c r="A207" s="2"/>
     </row>
     <row r="208" spans="1:7">
-      <c r="B208" s="2"/>
+      <c r="A208" s="2"/>
     </row>
     <row r="209" spans="1:7">
-      <c r="B209" s="2"/>
+      <c r="A209" s="2"/>
     </row>
     <row r="210" spans="1:7">
-      <c r="B210" s="2"/>
+      <c r="A210" s="2"/>
     </row>
     <row r="211" spans="1:7">
-      <c r="B211" s="2"/>
+      <c r="A211" s="2"/>
     </row>
     <row r="212" spans="1:7">
-      <c r="B212" s="2"/>
+      <c r="A212" s="2"/>
     </row>
     <row r="213" spans="1:7">
-      <c r="B213" s="2"/>
+      <c r="A213" s="2"/>
     </row>
     <row r="214" spans="1:7">
-      <c r="B214" s="2"/>
+      <c r="A214" s="2"/>
     </row>
     <row r="215" spans="1:7">
-      <c r="B215" s="2"/>
+      <c r="A215" s="2"/>
     </row>
     <row r="216" spans="1:7">
-      <c r="B216" s="2"/>
+      <c r="A216" s="2"/>
     </row>
     <row r="217" spans="1:7">
-      <c r="B217" s="2"/>
+      <c r="A217" s="2"/>
     </row>
     <row r="218" spans="1:7">
-      <c r="B218" s="2"/>
+      <c r="A218" s="2"/>
     </row>
     <row r="219" spans="1:7">
-      <c r="B219" s="2"/>
+      <c r="A219" s="2"/>
     </row>
     <row r="220" spans="1:7">
-      <c r="B220" s="2"/>
+      <c r="A220" s="2"/>
     </row>
     <row r="221" spans="1:7">
-      <c r="B221" s="2"/>
+      <c r="A221" s="2"/>
     </row>
     <row r="222" spans="1:7">
-      <c r="B222" s="2"/>
+      <c r="A222" s="2"/>
     </row>
     <row r="223" spans="1:7">
-      <c r="B223" s="2"/>
+      <c r="A223" s="2"/>
     </row>
     <row r="224" spans="1:7">
-      <c r="B224" s="2"/>
+      <c r="A224" s="2"/>
     </row>
     <row r="225" spans="1:7">
-      <c r="B225" s="2"/>
+      <c r="A225" s="2"/>
     </row>
     <row r="226" spans="1:7">
-      <c r="B226" s="2"/>
+      <c r="A226" s="2"/>
     </row>
     <row r="227" spans="1:7">
-      <c r="B227" s="2"/>
+      <c r="A227" s="2"/>
     </row>
     <row r="228" spans="1:7">
-      <c r="B228" s="2"/>
+      <c r="A228" s="2"/>
     </row>
     <row r="229" spans="1:7">
-      <c r="B229" s="2"/>
+      <c r="A229" s="2"/>
     </row>
     <row r="230" spans="1:7">
-      <c r="B230" s="2"/>
+      <c r="A230" s="2"/>
     </row>
     <row r="231" spans="1:7">
-      <c r="B231" s="2"/>
+      <c r="A231" s="2"/>
     </row>
     <row r="232" spans="1:7">
-      <c r="B232" s="2"/>
+      <c r="A232" s="2"/>
     </row>
     <row r="233" spans="1:7">
-      <c r="B233" s="2"/>
+      <c r="A233" s="2"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="B234" s="2"/>
+      <c r="A234" s="2"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="B235" s="2"/>
+      <c r="A235" s="2"/>
     </row>
     <row r="236" spans="1:7">
-      <c r="B236" s="2"/>
+      <c r="A236" s="2"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="B237" s="2"/>
+      <c r="A237" s="2"/>
     </row>
     <row r="238" spans="1:7">
-      <c r="B238" s="2"/>
+      <c r="A238" s="2"/>
     </row>
     <row r="239" spans="1:7">
-      <c r="B239" s="2"/>
+      <c r="A239" s="2"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="B240" s="2"/>
+      <c r="A240" s="2"/>
     </row>
     <row r="241" spans="1:7">
-      <c r="B241" s="2"/>
+      <c r="A241" s="2"/>
     </row>
     <row r="242" spans="1:7">
-      <c r="B242" s="2"/>
+      <c r="A242" s="2"/>
     </row>
     <row r="243" spans="1:7">
-      <c r="B243" s="2"/>
+      <c r="A243" s="2"/>
     </row>
     <row r="244" spans="1:7">
-      <c r="B244" s="2"/>
+      <c r="A244" s="2"/>
     </row>
     <row r="245" spans="1:7">
-      <c r="B245" s="2"/>
+      <c r="A245" s="2"/>
     </row>
     <row r="246" spans="1:7">
-      <c r="B246" s="2"/>
+      <c r="A246" s="2"/>
     </row>
     <row r="247" spans="1:7">
-      <c r="B247" s="2"/>
+      <c r="A247" s="2"/>
     </row>
     <row r="248" spans="1:7">
-      <c r="B248" s="2"/>
+      <c r="A248" s="2"/>
     </row>
     <row r="249" spans="1:7">
-      <c r="B249" s="2"/>
+      <c r="A249" s="2"/>
     </row>
     <row r="250" spans="1:7">
-      <c r="B250" s="2"/>
+      <c r="A250" s="2"/>
     </row>
     <row r="251" spans="1:7">
-      <c r="B251" s="2"/>
+      <c r="A251" s="2"/>
     </row>
     <row r="252" spans="1:7">
-      <c r="B252" s="2"/>
+      <c r="A252" s="2"/>
     </row>
     <row r="253" spans="1:7">
-      <c r="B253" s="2"/>
+      <c r="A253" s="2"/>
     </row>
     <row r="254" spans="1:7">
-      <c r="B254" s="2"/>
+      <c r="A254" s="2"/>
     </row>
     <row r="255" spans="1:7">
-      <c r="B255" s="2"/>
+      <c r="A255" s="2"/>
     </row>
     <row r="256" spans="1:7">
-      <c r="B256" s="2"/>
+      <c r="A256" s="2"/>
     </row>
     <row r="257" spans="1:7">
-      <c r="B257" s="2"/>
+      <c r="A257" s="2"/>
     </row>
     <row r="258" spans="1:7">
-      <c r="B258" s="2"/>
+      <c r="A258" s="2"/>
     </row>
     <row r="259" spans="1:7">
-      <c r="B259" s="2"/>
+      <c r="A259" s="2"/>
     </row>
     <row r="260" spans="1:7">
-      <c r="B260" s="2"/>
+      <c r="A260" s="2"/>
     </row>
     <row r="261" spans="1:7">
-      <c r="B261" s="2"/>
+      <c r="A261" s="2"/>
     </row>
     <row r="262" spans="1:7">
-      <c r="B262" s="2"/>
+      <c r="A262" s="2"/>
     </row>
     <row r="263" spans="1:7">
-      <c r="B263" s="2"/>
+      <c r="A263" s="2"/>
     </row>
     <row r="264" spans="1:7">
-      <c r="B264" s="2"/>
+      <c r="A264" s="2"/>
     </row>
     <row r="265" spans="1:7">
-      <c r="B265" s="2"/>
+      <c r="A265" s="2"/>
     </row>
     <row r="266" spans="1:7">
-      <c r="B266" s="2"/>
+      <c r="A266" s="2"/>
     </row>
     <row r="267" spans="1:7">
-      <c r="B267" s="2"/>
+      <c r="A267" s="2"/>
     </row>
     <row r="268" spans="1:7">
-      <c r="B268" s="2"/>
+      <c r="A268" s="2"/>
     </row>
     <row r="269" spans="1:7">
-      <c r="B269" s="2"/>
+      <c r="A269" s="2"/>
     </row>
     <row r="270" spans="1:7">
-      <c r="B270" s="2"/>
+      <c r="A270" s="2"/>
     </row>
     <row r="271" spans="1:7">
-      <c r="B271" s="2"/>
+      <c r="A271" s="2"/>
     </row>
     <row r="272" spans="1:7">
-      <c r="B272" s="2"/>
+      <c r="A272" s="2"/>
     </row>
     <row r="273" spans="1:7">
-      <c r="B273" s="2"/>
+      <c r="A273" s="2"/>
     </row>
     <row r="274" spans="1:7">
-      <c r="B274" s="2"/>
+      <c r="A274" s="2"/>
     </row>
     <row r="275" spans="1:7">
-      <c r="B275" s="2"/>
+      <c r="A275" s="2"/>
     </row>
     <row r="276" spans="1:7">
-      <c r="B276" s="2"/>
+      <c r="A276" s="2"/>
     </row>
     <row r="277" spans="1:7">
-      <c r="B277" s="2"/>
+      <c r="A277" s="2"/>
     </row>
     <row r="278" spans="1:7">
-      <c r="B278" s="2"/>
+      <c r="A278" s="2"/>
     </row>
     <row r="279" spans="1:7">
-      <c r="B279" s="2"/>
+      <c r="A279" s="2"/>
     </row>
     <row r="280" spans="1:7">
-      <c r="B280" s="2"/>
+      <c r="A280" s="2"/>
     </row>
     <row r="281" spans="1:7">
-      <c r="B281" s="2"/>
+      <c r="A281" s="2"/>
     </row>
     <row r="282" spans="1:7">
-      <c r="B282" s="2"/>
+      <c r="A282" s="2"/>
     </row>
     <row r="283" spans="1:7">
-      <c r="B283" s="2"/>
+      <c r="A283" s="2"/>
     </row>
     <row r="284" spans="1:7">
-      <c r="B284" s="2"/>
+      <c r="A284" s="2"/>
     </row>
     <row r="285" spans="1:7">
-      <c r="B285" s="2"/>
+      <c r="A285" s="2"/>
     </row>
     <row r="286" spans="1:7">
-      <c r="B286" s="2"/>
+      <c r="A286" s="2"/>
     </row>
     <row r="287" spans="1:7">
-      <c r="B287" s="2"/>
+      <c r="A287" s="2"/>
     </row>
     <row r="288" spans="1:7">
-      <c r="B288" s="2"/>
+      <c r="A288" s="2"/>
     </row>
     <row r="289" spans="1:7">
-      <c r="B289" s="2"/>
+      <c r="A289" s="2"/>
     </row>
     <row r="290" spans="1:7">
-      <c r="B290" s="2"/>
+      <c r="A290" s="2"/>
     </row>
     <row r="291" spans="1:7">
-      <c r="B291" s="2"/>
+      <c r="A291" s="2"/>
     </row>
     <row r="292" spans="1:7">
-      <c r="B292" s="2"/>
+      <c r="A292" s="2"/>
     </row>
     <row r="293" spans="1:7">
-      <c r="B293" s="2"/>
+      <c r="A293" s="2"/>
     </row>
     <row r="294" spans="1:7">
-      <c r="B294" s="2"/>
+      <c r="A294" s="2"/>
     </row>
     <row r="295" spans="1:7">
-      <c r="B295" s="2"/>
+      <c r="A295" s="2"/>
     </row>
     <row r="296" spans="1:7">
-      <c r="B296" s="2"/>
+      <c r="A296" s="2"/>
     </row>
     <row r="297" spans="1:7">
-      <c r="B297" s="2"/>
+      <c r="A297" s="2"/>
     </row>
     <row r="298" spans="1:7">
-      <c r="B298" s="2"/>
+      <c r="A298" s="2"/>
     </row>
     <row r="299" spans="1:7">
-      <c r="B299" s="2"/>
+      <c r="A299" s="2"/>
     </row>
     <row r="300" spans="1:7">
-      <c r="B300" s="2"/>
+      <c r="A300" s="2"/>
     </row>
     <row r="301" spans="1:7">
-      <c r="B301" s="2"/>
+      <c r="A301" s="2"/>
     </row>
     <row r="302" spans="1:7">
-      <c r="B302" s="2"/>
+      <c r="A302" s="2"/>
     </row>
     <row r="303" spans="1:7">
-      <c r="B303" s="2"/>
+      <c r="A303" s="2"/>
     </row>
     <row r="304" spans="1:7">
-      <c r="B304" s="2"/>
+      <c r="A304" s="2"/>
     </row>
     <row r="305" spans="1:7">
-      <c r="B305" s="2"/>
+      <c r="A305" s="2"/>
     </row>
     <row r="306" spans="1:7">
-      <c r="B306" s="2"/>
+      <c r="A306" s="2"/>
     </row>
     <row r="307" spans="1:7">
-      <c r="B307" s="2"/>
+      <c r="A307" s="2"/>
     </row>
     <row r="308" spans="1:7">
-      <c r="B308" s="2"/>
+      <c r="A308" s="2"/>
     </row>
     <row r="309" spans="1:7">
-      <c r="B309" s="2"/>
+      <c r="A309" s="2"/>
     </row>
     <row r="310" spans="1:7">
-      <c r="B310" s="2"/>
+      <c r="A310" s="2"/>
     </row>
     <row r="311" spans="1:7">
-      <c r="B311" s="2"/>
+      <c r="A311" s="2"/>
     </row>
     <row r="312" spans="1:7">
-      <c r="B312" s="2"/>
+      <c r="A312" s="2"/>
     </row>
     <row r="313" spans="1:7">
-      <c r="B313" s="2"/>
+      <c r="A313" s="2"/>
     </row>
     <row r="314" spans="1:7">
-      <c r="B314" s="2"/>
+      <c r="A314" s="2"/>
     </row>
     <row r="315" spans="1:7">
-      <c r="B315" s="2"/>
-    </row>
-    <row r="316" spans="1:7">
-      <c r="B316" s="2"/>
-    </row>
-    <row r="317" spans="1:7">
-      <c r="B317" s="2"/>
-    </row>
-    <row r="318" spans="1:7">
-      <c r="B318" s="2"/>
-    </row>
-    <row r="319" spans="1:7">
-      <c r="B319" s="2"/>
-    </row>
-    <row r="320" spans="1:7">
-      <c r="B320" s="2"/>
-    </row>
-    <row r="321" spans="1:7">
-      <c r="B321" s="2"/>
-    </row>
-    <row r="322" spans="1:7">
-      <c r="B322" s="2"/>
-    </row>
-    <row r="323" spans="1:7">
-      <c r="B323" s="2"/>
-    </row>
-    <row r="324" spans="1:7">
-      <c r="B324" s="2"/>
-    </row>
-    <row r="325" spans="1:7">
-      <c r="B325" s="2"/>
-    </row>
-    <row r="326" spans="1:7">
-      <c r="B326" s="2"/>
-    </row>
-    <row r="327" spans="1:7">
-      <c r="B327" s="2"/>
-    </row>
-    <row r="328" spans="1:7">
-      <c r="B328" s="2"/>
-    </row>
-    <row r="329" spans="1:7">
-      <c r="B329" s="2"/>
-    </row>
-    <row r="330" spans="1:7">
-      <c r="B330" s="2"/>
-    </row>
-    <row r="331" spans="1:7">
-      <c r="B331" s="2"/>
-    </row>
-    <row r="332" spans="1:7">
-      <c r="B332" s="2"/>
-    </row>
-    <row r="333" spans="1:7">
-      <c r="B333" s="2"/>
-    </row>
-    <row r="334" spans="1:7">
-      <c r="B334" s="2"/>
-    </row>
-    <row r="335" spans="1:7">
-      <c r="B335" s="2"/>
-    </row>
-    <row r="336" spans="1:7">
-      <c r="B336" s="2"/>
-    </row>
-    <row r="337" spans="1:7">
-      <c r="B337" s="2"/>
-    </row>
-    <row r="338" spans="1:7">
-      <c r="B338" s="2"/>
-    </row>
-    <row r="339" spans="1:7">
-      <c r="B339" s="2"/>
-    </row>
-    <row r="340" spans="1:7">
-      <c r="B340" s="2"/>
-    </row>
-    <row r="341" spans="1:7">
-      <c r="B341" s="2"/>
-    </row>
-    <row r="342" spans="1:7">
-      <c r="B342" s="2"/>
-    </row>
-    <row r="343" spans="1:7">
-      <c r="B343" s="2"/>
-    </row>
-    <row r="344" spans="1:7">
-      <c r="B344" s="2"/>
-    </row>
-    <row r="345" spans="1:7">
-      <c r="B345" s="2"/>
-    </row>
-    <row r="346" spans="1:7">
-      <c r="B346" s="2"/>
-    </row>
-    <row r="347" spans="1:7">
-      <c r="B347" s="2"/>
-    </row>
-    <row r="348" spans="1:7">
-      <c r="B348" s="2"/>
-    </row>
-    <row r="349" spans="1:7">
-      <c r="B349" s="2"/>
-    </row>
-    <row r="350" spans="1:7">
-      <c r="B350" s="2"/>
-    </row>
-    <row r="351" spans="1:7">
-      <c r="B351" s="2"/>
-    </row>
-    <row r="352" spans="1:7">
-      <c r="B352" s="2"/>
-    </row>
-    <row r="353" spans="1:7">
-      <c r="B353" s="2"/>
-    </row>
-    <row r="354" spans="1:7">
-      <c r="B354" s="2"/>
-    </row>
-    <row r="355" spans="1:7">
-      <c r="B355" s="2"/>
-    </row>
-    <row r="356" spans="1:7">
-      <c r="B356" s="2"/>
-    </row>
-    <row r="357" spans="1:7">
-      <c r="B357" s="2"/>
-    </row>
-    <row r="358" spans="1:7">
-      <c r="B358" s="2"/>
-    </row>
-    <row r="359" spans="1:7">
-      <c r="B359" s="2"/>
-    </row>
-    <row r="360" spans="1:7">
-      <c r="B360" s="2"/>
-    </row>
-    <row r="361" spans="1:7">
-      <c r="B361" s="2"/>
-    </row>
-    <row r="362" spans="1:7">
-      <c r="B362" s="2"/>
+      <c r="A315" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added arr and rev to ForecastTemplate
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/JASON/ForecastResult2017.xlsx
+++ b/Prototype/PHPSCRIPTS/JASON/ForecastResult2017.xlsx
@@ -10,15 +10,17 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="rns">'Sheet1'!$B$2:$B$7</definedName>
-    <definedName name="Timeline">'Sheet1'!$A$2:$A$7</definedName>
+    <definedName name="timeline">'Sheet1'!$A$2:$A$4</definedName>
+    <definedName name="rns">'Sheet1'!$B$2:$B$4</definedName>
+    <definedName name="arr">'Sheet1'!$C$2:$C$4</definedName>
+    <definedName name="rev">'Sheet1'!$D$2:$D$4</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Timeline</t>
   </si>
@@ -26,10 +28,22 @@
     <t>Room Nights Sold</t>
   </si>
   <si>
+    <t>Average Room Rate</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Forecasted Date</t>
   </si>
   <si>
-    <t>Forecast</t>
+    <t>Room Night Sold Forecast</t>
+  </si>
+  <si>
+    <t>Average Room Rate Forecast</t>
+  </si>
+  <si>
+    <t>Revenue Forecast</t>
   </si>
 </sst>
 </file>
@@ -379,10 +393,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G315"/>
+  <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -392,1008 +406,1030 @@
     <col min="3" max="3" width="19.28515625" customWidth="true" style="0"/>
     <col min="4" max="4" width="15.42578125" customWidth="true" style="0"/>
     <col min="5" max="5" width="10.85546875" customWidth="true" style="0"/>
-    <col min="6" max="6" width="7.42578125" customWidth="true" style="0"/>
-    <col min="7" max="7" width="8" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15.42578125" customWidth="true" style="0"/>
+    <col min="7" max="7" width="24" customWidth="true" style="0"/>
+    <col min="8" max="8" width="26.7109375" customWidth="true" style="0"/>
+    <col min="9" max="9" width="16.85546875" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="str">
-        <f>DATE(2016,07,31)</f>
+        <f>DATE(2016,10,31)</f>
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1100</v>
-      </c>
-      <c r="D2" t="str">
+        <v>1440</v>
+      </c>
+      <c r="C2">
+        <v>5703</v>
+      </c>
+      <c r="D2">
+        <v>8212</v>
+      </c>
+      <c r="F2" t="str">
         <f>EOMONTH(DATE(2016,12,31),1)</f>
         <v>0</v>
       </c>
-      <c r="E2" t="str">
-        <f>_xlfn.FORECAST.ETS($D2,rns,timeline,1,1)</f>
+      <c r="G2" t="str">
+        <f>_xlfn.FORECAST.ETS($F2,rns,timeline,1,1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="str">
+        <f>_xlfn.FORECAST.ETS($F2,arr,timeline,1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xlfn.FORECAST.ETS($F2,rev,timeline,1,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="str">
-        <f>DATE(2016,08,31)</f>
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="str">
-        <f>DATE(2016,09,30)</f>
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="str">
-        <f>DATE(2016,10,31)</f>
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="str">
         <f>DATE(2016,11,30)</f>
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B3">
         <v>1161</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="str">
+      <c r="C3">
+        <v>5852</v>
+      </c>
+      <c r="D3">
+        <v>6794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="str">
         <f>DATE(2016,12,31)</f>
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B4">
         <v>2686</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="C4">
+        <v>6452</v>
+      </c>
+      <c r="D4">
+        <v>17331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:9">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:9">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:9">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:9">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:9">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:9">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:9">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:9">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:9">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:9">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:9">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:9">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:9">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:9">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:9">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:9">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:9">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:9">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:9">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:9">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:9">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:9">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:9">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:9">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:9">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:9">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:9">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:9">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:9">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:9">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:9">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:9">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:9">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:9">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:9">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:9">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:9">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:9">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:9">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:9">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:9">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:9">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:9">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:9">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:9">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:9">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:9">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:9">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:9">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:9">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:9">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:9">
       <c r="A73" s="2"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:9">
       <c r="A74" s="2"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:9">
       <c r="A75" s="2"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:9">
       <c r="A76" s="2"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:9">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:9">
       <c r="A78" s="2"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:9">
       <c r="A79" s="2"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:9">
       <c r="A80" s="2"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:9">
       <c r="A81" s="2"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:9">
       <c r="A82" s="2"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:9">
       <c r="A83" s="2"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:9">
       <c r="A84" s="2"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:9">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:9">
       <c r="A86" s="2"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:9">
       <c r="A87" s="2"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:9">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:9">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:9">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:9">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:9">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:9">
       <c r="A93" s="2"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:9">
       <c r="A94" s="2"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:9">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:9">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:9">
       <c r="A97" s="2"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:9">
       <c r="A98" s="2"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:9">
       <c r="A99" s="2"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:9">
       <c r="A100" s="2"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:9">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:9">
       <c r="A102" s="2"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:9">
       <c r="A103" s="2"/>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:9">
       <c r="A104" s="2"/>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:9">
       <c r="A105" s="2"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:9">
       <c r="A106" s="2"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:9">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:9">
       <c r="A108" s="2"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:9">
       <c r="A109" s="2"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:9">
       <c r="A110" s="2"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:9">
       <c r="A111" s="2"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:9">
       <c r="A112" s="2"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:9">
       <c r="A113" s="2"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:9">
       <c r="A114" s="2"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:9">
       <c r="A115" s="2"/>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:9">
       <c r="A116" s="2"/>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:9">
       <c r="A117" s="2"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:9">
       <c r="A118" s="2"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:9">
       <c r="A119" s="2"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:9">
       <c r="A120" s="2"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:9">
       <c r="A121" s="2"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:9">
       <c r="A122" s="2"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:9">
       <c r="A123" s="2"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:9">
       <c r="A124" s="2"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:9">
       <c r="A125" s="2"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:9">
       <c r="A126" s="2"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:9">
       <c r="A127" s="2"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:9">
       <c r="A128" s="2"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:9">
       <c r="A129" s="2"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:9">
       <c r="A130" s="2"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:9">
       <c r="A131" s="2"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:9">
       <c r="A132" s="2"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:9">
       <c r="A133" s="2"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:9">
       <c r="A134" s="2"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:9">
       <c r="A135" s="2"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:9">
       <c r="A136" s="2"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:9">
       <c r="A137" s="2"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:9">
       <c r="A138" s="2"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:9">
       <c r="A139" s="2"/>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:9">
       <c r="A140" s="2"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:9">
       <c r="A141" s="2"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:9">
       <c r="A142" s="2"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:9">
       <c r="A143" s="2"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:9">
       <c r="A144" s="2"/>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:9">
       <c r="A145" s="2"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:9">
       <c r="A146" s="2"/>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:9">
       <c r="A147" s="2"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:9">
       <c r="A148" s="2"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:9">
       <c r="A149" s="2"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:9">
       <c r="A150" s="2"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:9">
       <c r="A151" s="2"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:9">
       <c r="A152" s="2"/>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:9">
       <c r="A153" s="2"/>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:9">
       <c r="A154" s="2"/>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:9">
       <c r="A155" s="2"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:9">
       <c r="A156" s="2"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:9">
       <c r="A157" s="2"/>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:9">
       <c r="A158" s="2"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:9">
       <c r="A159" s="2"/>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:9">
       <c r="A160" s="2"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:9">
       <c r="A161" s="2"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:9">
       <c r="A162" s="2"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:9">
       <c r="A163" s="2"/>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:9">
       <c r="A164" s="2"/>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:9">
       <c r="A165" s="2"/>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:9">
       <c r="A166" s="2"/>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:9">
       <c r="A167" s="2"/>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:9">
       <c r="A168" s="2"/>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:9">
       <c r="A169" s="2"/>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:9">
       <c r="A170" s="2"/>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:9">
       <c r="A171" s="2"/>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:9">
       <c r="A172" s="2"/>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:9">
       <c r="A173" s="2"/>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:9">
       <c r="A174" s="2"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:9">
       <c r="A175" s="2"/>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:9">
       <c r="A176" s="2"/>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:9">
       <c r="A177" s="2"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:9">
       <c r="A178" s="2"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:9">
       <c r="A179" s="2"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:9">
       <c r="A180" s="2"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:9">
       <c r="A181" s="2"/>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:9">
       <c r="A182" s="2"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:9">
       <c r="A183" s="2"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:9">
       <c r="A184" s="2"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:9">
       <c r="A185" s="2"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:9">
       <c r="A186" s="2"/>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:9">
       <c r="A187" s="2"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:9">
       <c r="A188" s="2"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:9">
       <c r="A189" s="2"/>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:9">
       <c r="A190" s="2"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:9">
       <c r="A191" s="2"/>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:9">
       <c r="A192" s="2"/>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:9">
       <c r="A193" s="2"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:9">
       <c r="A194" s="2"/>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:9">
       <c r="A195" s="2"/>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:9">
       <c r="A196" s="2"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:9">
       <c r="A197" s="2"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:9">
       <c r="A198" s="2"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:9">
       <c r="A199" s="2"/>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:9">
       <c r="A200" s="2"/>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:9">
       <c r="A201" s="2"/>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:9">
       <c r="A202" s="2"/>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:9">
       <c r="A203" s="2"/>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:9">
       <c r="A204" s="2"/>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:9">
       <c r="A205" s="2"/>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:9">
       <c r="A206" s="2"/>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:9">
       <c r="A207" s="2"/>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:9">
       <c r="A208" s="2"/>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:9">
       <c r="A209" s="2"/>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:9">
       <c r="A210" s="2"/>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:9">
       <c r="A211" s="2"/>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:9">
       <c r="A212" s="2"/>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:9">
       <c r="A213" s="2"/>
     </row>
-    <row r="214" spans="1:7">
+    <row r="214" spans="1:9">
       <c r="A214" s="2"/>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:9">
       <c r="A215" s="2"/>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:9">
       <c r="A216" s="2"/>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:9">
       <c r="A217" s="2"/>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:9">
       <c r="A218" s="2"/>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:9">
       <c r="A219" s="2"/>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:9">
       <c r="A220" s="2"/>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:9">
       <c r="A221" s="2"/>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:9">
       <c r="A222" s="2"/>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:9">
       <c r="A223" s="2"/>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:9">
       <c r="A224" s="2"/>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:9">
       <c r="A225" s="2"/>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:9">
       <c r="A226" s="2"/>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:9">
       <c r="A227" s="2"/>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:9">
       <c r="A228" s="2"/>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:9">
       <c r="A229" s="2"/>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:9">
       <c r="A230" s="2"/>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:9">
       <c r="A231" s="2"/>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:9">
       <c r="A232" s="2"/>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:9">
       <c r="A233" s="2"/>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:9">
       <c r="A234" s="2"/>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:9">
       <c r="A235" s="2"/>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:9">
       <c r="A236" s="2"/>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:9">
       <c r="A237" s="2"/>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:9">
       <c r="A238" s="2"/>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:9">
       <c r="A239" s="2"/>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:9">
       <c r="A240" s="2"/>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:9">
       <c r="A241" s="2"/>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:9">
       <c r="A242" s="2"/>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:9">
       <c r="A243" s="2"/>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:9">
       <c r="A244" s="2"/>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:9">
       <c r="A245" s="2"/>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:9">
       <c r="A246" s="2"/>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:9">
       <c r="A247" s="2"/>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:9">
       <c r="A248" s="2"/>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:9">
       <c r="A249" s="2"/>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:9">
       <c r="A250" s="2"/>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:9">
       <c r="A251" s="2"/>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:9">
       <c r="A252" s="2"/>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:9">
       <c r="A253" s="2"/>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:9">
       <c r="A254" s="2"/>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:9">
       <c r="A255" s="2"/>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:9">
       <c r="A256" s="2"/>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:9">
       <c r="A257" s="2"/>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:9">
       <c r="A258" s="2"/>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:9">
       <c r="A259" s="2"/>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:9">
       <c r="A260" s="2"/>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:9">
       <c r="A261" s="2"/>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:9">
       <c r="A262" s="2"/>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:9">
       <c r="A263" s="2"/>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:9">
       <c r="A264" s="2"/>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:9">
       <c r="A265" s="2"/>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:9">
       <c r="A266" s="2"/>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:9">
       <c r="A267" s="2"/>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:9">
       <c r="A268" s="2"/>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:9">
       <c r="A269" s="2"/>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:9">
       <c r="A270" s="2"/>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:9">
       <c r="A271" s="2"/>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:9">
       <c r="A272" s="2"/>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:9">
       <c r="A273" s="2"/>
     </row>
-    <row r="274" spans="1:7">
+    <row r="274" spans="1:9">
       <c r="A274" s="2"/>
     </row>
-    <row r="275" spans="1:7">
+    <row r="275" spans="1:9">
       <c r="A275" s="2"/>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:9">
       <c r="A276" s="2"/>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:9">
       <c r="A277" s="2"/>
     </row>
-    <row r="278" spans="1:7">
+    <row r="278" spans="1:9">
       <c r="A278" s="2"/>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:9">
       <c r="A279" s="2"/>
     </row>
-    <row r="280" spans="1:7">
+    <row r="280" spans="1:9">
       <c r="A280" s="2"/>
     </row>
-    <row r="281" spans="1:7">
+    <row r="281" spans="1:9">
       <c r="A281" s="2"/>
     </row>
-    <row r="282" spans="1:7">
+    <row r="282" spans="1:9">
       <c r="A282" s="2"/>
     </row>
-    <row r="283" spans="1:7">
+    <row r="283" spans="1:9">
       <c r="A283" s="2"/>
     </row>
-    <row r="284" spans="1:7">
+    <row r="284" spans="1:9">
       <c r="A284" s="2"/>
     </row>
-    <row r="285" spans="1:7">
+    <row r="285" spans="1:9">
       <c r="A285" s="2"/>
     </row>
-    <row r="286" spans="1:7">
+    <row r="286" spans="1:9">
       <c r="A286" s="2"/>
     </row>
-    <row r="287" spans="1:7">
+    <row r="287" spans="1:9">
       <c r="A287" s="2"/>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:9">
       <c r="A288" s="2"/>
     </row>
-    <row r="289" spans="1:7">
+    <row r="289" spans="1:9">
       <c r="A289" s="2"/>
     </row>
-    <row r="290" spans="1:7">
+    <row r="290" spans="1:9">
       <c r="A290" s="2"/>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:9">
       <c r="A291" s="2"/>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:9">
       <c r="A292" s="2"/>
     </row>
-    <row r="293" spans="1:7">
+    <row r="293" spans="1:9">
       <c r="A293" s="2"/>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:9">
       <c r="A294" s="2"/>
     </row>
-    <row r="295" spans="1:7">
+    <row r="295" spans="1:9">
       <c r="A295" s="2"/>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:9">
       <c r="A296" s="2"/>
     </row>
-    <row r="297" spans="1:7">
+    <row r="297" spans="1:9">
       <c r="A297" s="2"/>
     </row>
-    <row r="298" spans="1:7">
+    <row r="298" spans="1:9">
       <c r="A298" s="2"/>
     </row>
-    <row r="299" spans="1:7">
+    <row r="299" spans="1:9">
       <c r="A299" s="2"/>
     </row>
-    <row r="300" spans="1:7">
+    <row r="300" spans="1:9">
       <c r="A300" s="2"/>
     </row>
-    <row r="301" spans="1:7">
+    <row r="301" spans="1:9">
       <c r="A301" s="2"/>
     </row>
-    <row r="302" spans="1:7">
+    <row r="302" spans="1:9">
       <c r="A302" s="2"/>
     </row>
-    <row r="303" spans="1:7">
+    <row r="303" spans="1:9">
       <c r="A303" s="2"/>
     </row>
-    <row r="304" spans="1:7">
+    <row r="304" spans="1:9">
       <c r="A304" s="2"/>
     </row>
-    <row r="305" spans="1:7">
+    <row r="305" spans="1:9">
       <c r="A305" s="2"/>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:9">
       <c r="A306" s="2"/>
     </row>
-    <row r="307" spans="1:7">
+    <row r="307" spans="1:9">
       <c r="A307" s="2"/>
     </row>
-    <row r="308" spans="1:7">
+    <row r="308" spans="1:9">
       <c r="A308" s="2"/>
     </row>
-    <row r="309" spans="1:7">
+    <row r="309" spans="1:9">
       <c r="A309" s="2"/>
     </row>
-    <row r="310" spans="1:7">
+    <row r="310" spans="1:9">
       <c r="A310" s="2"/>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:9">
       <c r="A311" s="2"/>
     </row>
-    <row r="312" spans="1:7">
+    <row r="312" spans="1:9">
       <c r="A312" s="2"/>
     </row>
-    <row r="313" spans="1:7">
+    <row r="313" spans="1:9">
       <c r="A313" s="2"/>
     </row>
-    <row r="314" spans="1:7">
+    <row r="314" spans="1:9">
       <c r="A314" s="2"/>
     </row>
-    <row r="315" spans="1:7">
+    <row r="315" spans="1:9">
       <c r="A315" s="2"/>
     </row>
   </sheetData>

</xml_diff>